<commit_message>
Uploaded proper file for BulkUpload sample
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26404"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{350E043D-D222-463E-BA68-51E259736FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C901F2-A016-4E0E-B97E-06F03226D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,24 +35,60 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{34B5A6C4-93BC-4202-B7B9-FF39DAEE842A}">
       <text>
-        <t xml:space="preserve">Email Id for the user.
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Email Id for the user.
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DDB40CBC-1896-4134-9341-7093D58D2749}">
       <text>
-        <t>Mobile Number of the User</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Mobile Number of the User</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{43D12F7C-85CF-4C3B-B674-173B6B7C2871}">
       <text>
-        <t>Once the record is processed - the status will be updated in this column. 
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Once the record is processed - the status will be updated in this column. 
 Status would be SUCCESS / FAILED.</t>
+        </r>
       </text>
     </comment>
     <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D59FB896-8C6D-4D96-9130-0C1754D6D65D}">
       <text>
-        <t>If there is any error to create the user the error details would be updated in this column.</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>If there is any error to create the user the error details would be updated in this column.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -60,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>First Name</t>
   </si>
@@ -78,16 +114,42 @@
   </si>
   <si>
     <t>Error Details</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>ramesh.kumar@yopmail.com</t>
+  </si>
+  <si>
+    <t>Gita</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>gita.ben@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,15 +199,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,14 +526,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
@@ -495,18 +560,34 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9876543210</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9012345678</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
@@ -535,7 +616,11 @@
       <c r="F6" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{280A44BA-9B49-4416-81B8-9A00D06CC2ED}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{082F8A2C-2E0E-4E7B-9B38-B4C7C69ED955}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sample bulk upload file
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C901F2-A016-4E0E-B97E-06F03226D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IGOT\NIC\sunbird-cb-portal-assets\MDO\client-assets\assets\common\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2FBA6-9441-4760-9FA3-BE1CC56EDFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="5556" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +38,7 @@
     <author>Karthikeyan Rajendran</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{34B5A6C4-93BC-4202-B7B9-FF39DAEE842A}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{AFB07BED-1FC8-4D11-AD29-217F00DFC567}">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DDB40CBC-1896-4134-9341-7093D58D2749}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B67DCAC6-F5D7-4A7E-9E15-750A93421A90}">
       <text>
         <r>
           <rPr>
@@ -62,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{43D12F7C-85CF-4C3B-B674-173B6B7C2871}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{182F986D-585E-4DAE-B789-D828B926FAA7}">
       <text>
         <r>
           <rPr>
@@ -77,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D59FB896-8C6D-4D96-9130-0C1754D6D65D}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3B207D14-ECB2-43C5-A3B5-61D78FF60E8F}">
       <text>
         <r>
           <rPr>
@@ -138,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +151,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEDEDED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,18 +190,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,23 +510,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,66 +546,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>9876543210</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>9012345678</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{280A44BA-9B49-4416-81B8-9A00D06CC2ED}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{082F8A2C-2E0E-4E7B-9B38-B4C7C69ED955}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{718E1908-A3ED-4CB6-B530-B4E62702BFB5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{ECE8344A-B17E-4C17-9DAF-BF636214F48E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Bulk upload sample file format changes
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-bulk-upload-sample.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IGOT\NIC\sunbird-cb-portal-assets\MDO\client-assets\assets\common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2FBA6-9441-4760-9FA3-BE1CC56EDFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AC70103-5F32-4C26-8C8C-0FD2560511A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="5556" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7311328C-3CC2-4382-A573-CD63A7AF875D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,124 +35,51 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Karthikeyan Rajendran</author>
-  </authors>
-  <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{AFB07BED-1FC8-4D11-AD29-217F00DFC567}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">Email Id for the user.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B67DCAC6-F5D7-4A7E-9E15-750A93421A90}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Mobile Number of the User</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{182F986D-585E-4DAE-B789-D828B926FAA7}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Once the record is processed - the status will be updated in this column. 
-Status would be SUCCESS / FAILED.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3B207D14-ECB2-43C5-A3B5-61D78FF60E8F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>If there is any error to create the user the error details would be updated in this column.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>External Reference ID</t>
+  </si>
+  <si>
+    <t>External Reference System</t>
+  </si>
   <si>
     <t>First Name</t>
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t>Email Id</t>
-  </si>
-  <si>
-    <t>Mobile Number</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Error Details</t>
-  </si>
-  <si>
-    <t>Ramesh</t>
-  </si>
-  <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>ramesh.kumar@yopmail.com</t>
-  </si>
-  <si>
-    <t>Gita</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>gita.ben@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +92,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -176,16 +106,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -195,13 +125,13 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,77 +439,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AB659A-788E-42FA-AA49-4E47406AB9C7}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E409" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>9876543210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>9012345678</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{718E1908-A3ED-4CB6-B530-B4E62702BFB5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{ECE8344A-B17E-4C17-9DAF-BF636214F48E}"/>
-  </hyperlinks>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E421" xr:uid="{8BD4366F-DACE-4453-B467-284AE2FFDFD3}">
+      <formula1>"Group A,Group B,Group C,Group D,Contractual Staff, Others"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>